<commit_message>
Add a record row fot the number of redo
</commit_message>
<xml_diff>
--- a/力扣打卡记录 - 模板.xlsx
+++ b/力扣打卡记录 - 模板.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050EDABE-0BB4-4D7B-B5FF-A9D45441827C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9C178C-7C05-418B-9B57-42132C5A96A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="300" windowWidth="30936" windowHeight="17124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,11 +11,20 @@
     <sheet name="打卡模板" sheetId="38" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,13 +107,99 @@
   <si>
     <t>平均耗时/min</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重做次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+  </si>
+  <si>
+    <t>405. 数字转换为十六进制数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+  </si>
+  <si>
+    <t>超时通过</t>
+  </si>
+  <si>
+    <t>进制转换、位运算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 模拟+进制转化（先 % 后 /）1.1 包括处理负数的偏移量（使用 long 等更大的数据类型）   1.2 string 类型是顺序存储，尽量在尾部插入，最后再 reverse 逆转   2. 由数字转化为字符和字母（(char)(5+'0')）3. 位运算+分组换算 (num&gt;&gt;(i*4)) &amp; 0xf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已巩固</t>
+  </si>
+  <si>
+    <t>扩展开来，通过位运算+分组计算求任意进制的转化（如：10进制转化为 2进制(num &gt;&gt; i) &amp; 1、8进制(num &gt;&gt; (i*3)) &amp; 0x7、16进制的字符串(num &gt;&gt; (i*4)) &amp; 0xf）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已学习</t>
+  </si>
+  <si>
+    <t>通过</t>
+  </si>
+  <si>
+    <t>待学习</t>
+  </si>
+  <si>
+    <t>166. 分数到小数</t>
+  </si>
+  <si>
+    <t>中等</t>
+  </si>
+  <si>
+    <t>哈希</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 模拟竖式计算（除法）每次后补0继续除，直到循环或者除到0 2. 首先是涉及到负数转化为正数的，可能会溢出的，直接在一开始将入参转化为 long long 方便一点，3. 判断乘除正负号 可以通过 (numerator &lt; 0) ^ (denominator &lt; 0) 判断（注意 出现 0 的情况需要单独判断！！！）4. string 的 substr 和 insert 详细用法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>352. 将数据流变为多个不相交区间</t>
+  </si>
+  <si>
+    <t>困难</t>
+  </si>
+  <si>
+    <t>设计、二分查找、有序集合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. upper_bound() lower_bound() 二分查找函数 2. 二维 vector 插入 vector的语法 intervals.emplace_back(vector&lt;int&gt;{val, val}); intervals.insert(intervals.begin() + i, {val, val});</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待巩固</t>
+  </si>
+  <si>
+    <t>434. 字符串中的单词数</t>
+  </si>
+  <si>
+    <t>字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示后通过</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +242,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -173,7 +276,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -195,21 +298,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="56">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -271,6 +434,23 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -286,6 +466,245 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00AF9B"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFB800"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00AF9B"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFB800"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00AF9B"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFB800"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00AF9B"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFB800"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -531,8 +950,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.6614535653117087E-2"/>
-                  <c:y val="-0.21348279029585207"/>
+                  <c:x val="-0.13025423549418219"/>
+                  <c:y val="0.16411270345518472"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -657,16 +1076,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1688,16 +2107,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2C6781-4CF5-40F6-8069-6C29BB48CB57}">
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
@@ -1707,9 +2126,10 @@
     <col min="9" max="9" width="29.44140625" customWidth="1"/>
     <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1743,358 +2163,476 @@
       <c r="K1" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44531</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="E2" s="2"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="6">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44532</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="E3" s="2"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="6">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44533</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44534</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="6">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44535</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="9"/>
+      <c r="I6" s="7"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44536</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="9"/>
+      <c r="I7" s="7"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44537</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="9"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44538</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="9"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44539</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="7"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="9"/>
+      <c r="I10" s="7"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44540</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="9"/>
+      <c r="I11" s="7"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44541</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="9"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44542</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="G13" s="9"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="9"/>
+      <c r="I13" s="7"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44543</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="G14" s="9"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="9"/>
+      <c r="I14" s="7"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44544</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="9"/>
+      <c r="I15" s="7"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44545</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="G16" s="9"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="9"/>
+      <c r="I16" s="7"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44546</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="G17" s="9"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="9"/>
+      <c r="I17" s="7"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44547</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="G18" s="9"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="9"/>
+      <c r="I18" s="7"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44548</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="G19" s="9"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="7"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44549</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="G20" s="9"/>
+      <c r="G20" s="7"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="9"/>
+      <c r="I20" s="7"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44550</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="G21" s="9"/>
+      <c r="G21" s="7"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="9"/>
+      <c r="I21" s="7"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44551</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="G22" s="9"/>
+      <c r="G22" s="7"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="9"/>
+      <c r="I22" s="7"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44552</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="G23" s="9"/>
+      <c r="G23" s="7"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="9"/>
+      <c r="I23" s="7"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44553</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="G24" s="9"/>
+      <c r="G24" s="7"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="9"/>
+      <c r="I24" s="7"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44554</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="G25" s="9"/>
+      <c r="G25" s="7"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="9"/>
+      <c r="I25" s="7"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44555</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="G26" s="9"/>
+      <c r="G26" s="7"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="9"/>
+      <c r="I26" s="7"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44556</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="G27" s="9"/>
+      <c r="G27" s="7"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="9"/>
+      <c r="I27" s="7"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44557</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="G28" s="9"/>
+      <c r="G28" s="7"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="9"/>
+      <c r="I28" s="7"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44558</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="G29" s="9"/>
+      <c r="G29" s="7"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="9"/>
+      <c r="I29" s="7"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44559</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="G30" s="9"/>
+      <c r="G30" s="7"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="9"/>
+      <c r="I30" s="7"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44560</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="G31" s="9"/>
+      <c r="G31" s="7"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="9"/>
+      <c r="I31" s="7"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44561</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="G32" s="9"/>
+      <c r="G32" s="7"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="9"/>
+      <c r="I32" s="7"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
+      <c r="L32" s="6"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
     <row r="35" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="5"/>
+      <c r="B35" s="9"/>
       <c r="D35" s="4" t="s">
         <v>18</v>
       </c>
@@ -2109,18 +2647,18 @@
       </c>
       <c r="B36">
         <f>COUNTIF(C2:C32,"简单")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E36">
         <f>COUNTIF(D2:D32,"通过")</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="G36" s="10">
         <f>ROUND(AVERAGE(E2:E32), 0)</f>
-        <v>#DIV/0!</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2129,16 +2667,16 @@
       </c>
       <c r="B37">
         <f>COUNTIF(C2:C32,"中等")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E37">
         <f>COUNTIF(D2:D32,"超时通过")</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -2146,16 +2684,16 @@
       </c>
       <c r="B38">
         <f>COUNTIF(C2:C32,"困难")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E38">
         <f>COUNTIF(D2:D32,"提示后通过")</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -2164,57 +2702,57 @@
       </c>
       <c r="E39">
         <f>COUNTIF(D2:D32,"CV-未通过")</f>
-        <v>0</v>
-      </c>
-      <c r="G39" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
@@ -2302,76 +2840,200 @@
     <mergeCell ref="A42:G45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C31 C46:C1048576 C37:C39">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+  <conditionalFormatting sqref="C1 C46:C1048576 C37:C39 C6:C31">
+    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
       <formula>"中等"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
       <formula>"困难"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="63" operator="equal">
       <formula>"简单"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E31">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="E6:E31">
+    <cfRule type="cellIs" dxfId="52" priority="60" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G6:H31">
+    <cfRule type="expression" dxfId="51" priority="58">
+      <formula>$H6="待巩固"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:J31">
+    <cfRule type="expression" dxfId="50" priority="56">
+      <formula>$J6="待学习"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6:K31">
+    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
+      <formula>"是"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
+      <formula>"中等"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
+      <formula>"困难"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="54" operator="equal">
+      <formula>"简单"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="cellIs" dxfId="45" priority="51" operator="greaterThan">
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32:H32">
+    <cfRule type="expression" dxfId="44" priority="50">
+      <formula>$H32="待巩固"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32:J32">
+    <cfRule type="expression" dxfId="43" priority="49">
+      <formula>$J32="待学习"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
+    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
+      <formula>"是"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+      <formula>"中等"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+      <formula>"困难"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+      <formula>"简单"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="greaterThan">
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G2:H2">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="35" priority="36">
       <formula>$H2="待巩固"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H31">
-    <cfRule type="expression" dxfId="10" priority="11">
+  <conditionalFormatting sqref="I2:J2">
+    <cfRule type="expression" dxfId="34" priority="35">
+      <formula>$J2="待学习"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
+      <formula>"是"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
+      <formula>"中等"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+      <formula>"困难"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
+      <formula>"简单"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="greaterThan">
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:H3">
+    <cfRule type="expression" dxfId="26" priority="27">
       <formula>$H3="待巩固"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J2">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>$J2="待学习"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:J31">
+  <conditionalFormatting sqref="I3:J3">
+    <cfRule type="expression" dxfId="25" priority="26">
+      <formula>$J3="待学习"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+      <formula>"是"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+      <formula>"中等"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+      <formula>"困难"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
+      <formula>"简单"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:H4">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>$H4="待巩固"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:J4">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>$J4="待学习"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+      <formula>"是"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+      <formula>"中等"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>"困难"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+      <formula>"简单"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:H5">
     <cfRule type="expression" dxfId="8" priority="9">
-      <formula>$J3="待学习"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K31">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>$H5="待巩固"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:J5">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>$J5="待学习"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"是"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
-      <formula>"中等"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"困难"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
-      <formula>"简单"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
-      <formula>30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32:H32">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$H32="待巩固"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32:J32">
+  <conditionalFormatting sqref="L2:L32">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$J32="待学习"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"是"</formula>
+      <formula>AND($K2="是",$L2=2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L32">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND($K2="是",$L2&lt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -2394,8 +3056,13 @@
       <formula1>"自己做出,CV,看思路写出"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://leetcode-cn.com/problems/fraction-to-recurring-decimal/" xr:uid="{8D51DA5F-1B41-41CE-B03A-EAECF1E0D932}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{0BD7FB1E-91EE-47AC-A205-64343FC13F58}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://leetcode-cn.com/problems/number-of-segments-in-a-string/" xr:uid="{EA430F9D-A14D-4CDE-8359-A85C85DEB363}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the remarks column and changed the population of some columns to general
</commit_message>
<xml_diff>
--- a/力扣打卡记录 - 模板.xlsx
+++ b/力扣打卡记录 - 模板.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9C178C-7C05-418B-9B57-42132C5A96A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF89A6B3-2AC0-460C-A863-CB8807CF408E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="300" windowWidth="30936" windowHeight="17124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -193,6 +193,10 @@
   </si>
   <si>
     <t>提示后通过</t>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -276,7 +280,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -298,11 +302,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -316,12 +320,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="44">
     <dxf>
       <fill>
         <patternFill>
@@ -348,13 +355,48 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00AF9B"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFB800"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -365,13 +407,48 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00AF9B"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFB800"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -434,23 +511,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -493,161 +553,6 @@
       <font>
         <color rgb="FFFFB800"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00AF9B"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFB800"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00AF9B"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFB800"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1747,13 +1652,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>8459</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>11633</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>602429</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>80458</xdr:rowOff>
@@ -2107,7 +2012,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2C6781-4CF5-40F6-8069-6C29BB48CB57}">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -2129,7 +2034,7 @@
     <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2166,8 +2071,11 @@
       <c r="L1" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44531</v>
       </c>
@@ -2186,13 +2094,13 @@
       <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="13" t="s">
         <v>27</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="13" t="s">
         <v>29</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -2205,11 +2113,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44532</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -2224,13 +2132,13 @@
       <c r="F3" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="13" t="s">
         <v>36</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
         <v>44</v>
@@ -2239,7 +2147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44533</v>
       </c>
@@ -2258,9 +2166,9 @@
       <c r="F4" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="13" t="s">
         <v>40</v>
       </c>
       <c r="J4" s="6" t="s">
@@ -2273,11 +2181,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44534</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -2292,143 +2200,143 @@
       <c r="F5" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="13"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44535</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="G6" s="7"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="13"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44536</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="7"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44537</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="13"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44538</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="G9" s="7"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="7"/>
+      <c r="I9" s="13"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44539</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="13"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="13"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44540</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44541</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="7"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44542</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="13"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="7"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44543</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="7"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44544</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="7"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44545</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="13"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="7"/>
+      <c r="I16" s="13"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="6"/>
@@ -2438,9 +2346,9 @@
         <v>44546</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="7"/>
+      <c r="I17" s="13"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="6"/>
@@ -2450,9 +2358,9 @@
         <v>44547</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="7"/>
+      <c r="I18" s="13"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="6"/>
@@ -2462,9 +2370,9 @@
         <v>44548</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="G19" s="7"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="7"/>
+      <c r="I19" s="13"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="6"/>
@@ -2474,9 +2382,9 @@
         <v>44549</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="G20" s="7"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="7"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="6"/>
@@ -2486,9 +2394,9 @@
         <v>44550</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="G21" s="7"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="7"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="6"/>
@@ -2498,9 +2406,9 @@
         <v>44551</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="G22" s="7"/>
+      <c r="G22" s="13"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="7"/>
+      <c r="I22" s="13"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="6"/>
@@ -2510,9 +2418,9 @@
         <v>44552</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="G23" s="7"/>
+      <c r="G23" s="13"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="7"/>
+      <c r="I23" s="13"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="6"/>
@@ -2522,9 +2430,9 @@
         <v>44553</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="G24" s="7"/>
+      <c r="G24" s="13"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="7"/>
+      <c r="I24" s="13"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="6"/>
@@ -2534,9 +2442,9 @@
         <v>44554</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="G25" s="7"/>
+      <c r="G25" s="13"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="7"/>
+      <c r="I25" s="13"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="6"/>
@@ -2546,9 +2454,9 @@
         <v>44555</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="G26" s="7"/>
+      <c r="G26" s="13"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="7"/>
+      <c r="I26" s="13"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="6"/>
@@ -2558,9 +2466,9 @@
         <v>44556</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="G27" s="7"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="7"/>
+      <c r="I27" s="13"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="6"/>
@@ -2570,9 +2478,9 @@
         <v>44557</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="G28" s="7"/>
+      <c r="G28" s="13"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="7"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="6"/>
@@ -2582,9 +2490,9 @@
         <v>44558</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="G29" s="7"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="7"/>
+      <c r="I29" s="13"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="6"/>
@@ -2594,9 +2502,9 @@
         <v>44559</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="G30" s="7"/>
+      <c r="G30" s="13"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="7"/>
+      <c r="I30" s="13"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="6"/>
@@ -2606,9 +2514,9 @@
         <v>44560</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="G31" s="7"/>
+      <c r="G31" s="13"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="7"/>
+      <c r="I31" s="13"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="6"/>
@@ -2618,9 +2526,9 @@
         <v>44561</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="G32" s="7"/>
+      <c r="G32" s="13"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="7"/>
+      <c r="I32" s="13"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="6"/>
@@ -2841,188 +2749,188 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1 C46:C1048576 C37:C39 C6:C31">
-    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="61" operator="equal">
       <formula>"中等"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="62" operator="equal">
       <formula>"困难"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="63" operator="equal">
       <formula>"简单"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E31">
-    <cfRule type="cellIs" dxfId="52" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="60" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:H31">
-    <cfRule type="expression" dxfId="51" priority="58">
-      <formula>$H6="待巩固"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6:J31">
-    <cfRule type="expression" dxfId="50" priority="56">
-      <formula>$J6="待学习"</formula>
+  <conditionalFormatting sqref="G6:H31 G2:G32">
+    <cfRule type="expression" dxfId="39" priority="58">
+      <formula>$H2="待巩固"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:J31 I2:I32">
+    <cfRule type="expression" dxfId="38" priority="56">
+      <formula>$J2="待学习"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:K31">
-    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="55" operator="equal">
       <formula>"是"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="52" operator="equal">
       <formula>"中等"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="53" operator="equal">
       <formula>"困难"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="54" operator="equal">
       <formula>"简单"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="45" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="51" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:H32">
-    <cfRule type="expression" dxfId="44" priority="50">
+    <cfRule type="expression" dxfId="32" priority="50">
       <formula>$H32="待巩固"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:J32">
-    <cfRule type="expression" dxfId="43" priority="49">
+    <cfRule type="expression" dxfId="31" priority="49">
       <formula>$J32="待学习"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="48" operator="equal">
       <formula>"是"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
       <formula>"中等"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
       <formula>"困难"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="40" operator="equal">
       <formula>"简单"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:H2">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="25" priority="36">
       <formula>$H2="待巩固"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J2">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="24" priority="35">
       <formula>$J2="待学习"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
       <formula>"是"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="29" operator="equal">
       <formula>"中等"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
       <formula>"困难"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="31" operator="equal">
       <formula>"简单"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="28" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:H3">
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="18" priority="27">
       <formula>$H3="待巩固"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J3">
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="17" priority="26">
       <formula>$J3="待学习"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="25" operator="equal">
       <formula>"是"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
       <formula>"中等"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
       <formula>"困难"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
       <formula>"简单"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="19" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H4">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="11" priority="18">
       <formula>$H4="待巩固"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="10" priority="17">
       <formula>$J4="待学习"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="16" operator="equal">
       <formula>"是"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"中等"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>"困难"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"简单"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:H5">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>$H5="待巩固"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>$J5="待学习"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"是"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Modify some details of the template
</commit_message>
<xml_diff>
--- a/力扣打卡记录 - 模板.xlsx
+++ b/力扣打卡记录 - 模板.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF89A6B3-2AC0-460C-A863-CB8807CF408E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21BEB76-BE7F-4EDA-B7EC-B8A7E7DF625D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="300" windowWidth="30936" windowHeight="17124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,10 +69,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>待学知识</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>状态</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -196,6 +192,49 @@
   </si>
   <si>
     <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复习知识</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 两数相加</t>
+  </si>
+  <si>
+    <t>递归、链表、数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 二分 + 朴素维护区间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>159. 至多包含两个不同字符的最长子串</t>
+  </si>
+  <si>
+    <t>哈希表、滑动窗口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>160. 相交链表</t>
+  </si>
+  <si>
+    <t>哈希表、链表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>161. 相隔为 1 的编辑距离</t>
+  </si>
+  <si>
+    <t>双指针、字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>162. 寻找峰值</t>
+  </si>
+  <si>
+    <t>数组、二分查找</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -263,13 +302,22 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="2">
@@ -280,7 +328,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -308,6 +356,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -319,9 +373,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -855,8 +906,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.13025423549418219"/>
-                  <c:y val="0.16411270345518472"/>
+                  <c:x val="-0.1720740808689496"/>
+                  <c:y val="-4.7803189144566688E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -981,10 +1032,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -2015,7 +2066,7 @@
   <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2099,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>9</v>
@@ -2057,22 +2108,22 @@
         <v>10</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2080,34 +2131,34 @@
         <v>44531</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="6">
         <v>14</v>
       </c>
       <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="K2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L2" s="6">
         <v>2</v>
@@ -2118,30 +2169,30 @@
         <v>44532</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="6">
         <v>60</v>
       </c>
       <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>36</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="I3" s="9"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3" s="6">
         <v>3</v>
@@ -2152,30 +2203,32 @@
         <v>44533</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="10"/>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="13" t="s">
-        <v>40</v>
-      </c>
       <c r="J4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4" s="6">
         <v>1</v>
@@ -2186,23 +2239,23 @@
         <v>44534</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="6">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="13"/>
+        <v>42</v>
+      </c>
+      <c r="G5" s="9"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="13"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6">
@@ -2213,10 +2266,24 @@
       <c r="A6" s="1">
         <v>44535</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="G6" s="13"/>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="9"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="13"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="6"/>
@@ -2225,10 +2292,24 @@
       <c r="A7" s="1">
         <v>44536</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="G7" s="13"/>
+      <c r="B7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="9"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="13"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="6"/>
@@ -2237,10 +2318,24 @@
       <c r="A8" s="1">
         <v>44537</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="G8" s="13"/>
+      <c r="B8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="9"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="13"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="6"/>
@@ -2249,22 +2344,54 @@
       <c r="A9" s="1">
         <v>44538</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="9"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="13"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="6"/>
+      <c r="K9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44539</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="G10" s="13"/>
+      <c r="B10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="9"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="13"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="6"/>
@@ -2274,9 +2401,9 @@
         <v>44540</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="13"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="6"/>
@@ -2286,9 +2413,9 @@
         <v>44541</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="G12" s="13"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="13"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="6"/>
@@ -2298,9 +2425,9 @@
         <v>44542</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="G13" s="13"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="13"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="6"/>
@@ -2310,9 +2437,9 @@
         <v>44543</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="13"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="6"/>
@@ -2322,9 +2449,9 @@
         <v>44544</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="13"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="6"/>
@@ -2334,9 +2461,9 @@
         <v>44545</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="13"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="6"/>
@@ -2346,9 +2473,9 @@
         <v>44546</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="13"/>
+      <c r="I17" s="9"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="6"/>
@@ -2358,9 +2485,9 @@
         <v>44547</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="13"/>
+      <c r="I18" s="9"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="6"/>
@@ -2370,9 +2497,9 @@
         <v>44548</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="G19" s="13"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="13"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="6"/>
@@ -2382,9 +2509,9 @@
         <v>44549</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="G20" s="13"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="13"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="6"/>
@@ -2394,9 +2521,9 @@
         <v>44550</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="G21" s="13"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="13"/>
+      <c r="I21" s="9"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="6"/>
@@ -2406,9 +2533,9 @@
         <v>44551</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="G22" s="13"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="13"/>
+      <c r="I22" s="9"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="6"/>
@@ -2418,9 +2545,9 @@
         <v>44552</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="G23" s="13"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="13"/>
+      <c r="I23" s="9"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="6"/>
@@ -2430,9 +2557,9 @@
         <v>44553</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="G24" s="13"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="13"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="6"/>
@@ -2442,9 +2569,9 @@
         <v>44554</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="G25" s="13"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="13"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="6"/>
@@ -2454,9 +2581,9 @@
         <v>44555</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="G26" s="13"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="13"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="6"/>
@@ -2466,9 +2593,9 @@
         <v>44556</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="G27" s="13"/>
+      <c r="G27" s="9"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="13"/>
+      <c r="I27" s="9"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="6"/>
@@ -2478,9 +2605,9 @@
         <v>44557</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="G28" s="13"/>
+      <c r="G28" s="9"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="13"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="6"/>
@@ -2490,9 +2617,9 @@
         <v>44558</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="G29" s="13"/>
+      <c r="G29" s="9"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="13"/>
+      <c r="I29" s="9"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="6"/>
@@ -2502,9 +2629,9 @@
         <v>44559</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="G30" s="13"/>
+      <c r="G30" s="9"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="13"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="6"/>
@@ -2514,9 +2641,9 @@
         <v>44560</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="G31" s="13"/>
+      <c r="G31" s="9"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="13"/>
+      <c r="I31" s="9"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="6"/>
@@ -2526,9 +2653,9 @@
         <v>44561</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="G32" s="13"/>
+      <c r="G32" s="9"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="13"/>
+      <c r="I32" s="9"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="6"/>
@@ -2537,16 +2664,16 @@
       <c r="A33" s="1"/>
     </row>
     <row r="35" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="D35" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="G35" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="D35" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2555,18 +2682,18 @@
       </c>
       <c r="B36">
         <f>COUNTIF(C2:C32,"简单")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36">
         <f>COUNTIF(D2:D32,"通过")</f>
-        <v>1</v>
-      </c>
-      <c r="G36" s="10">
+        <v>5</v>
+      </c>
+      <c r="G36" s="12">
         <f>ROUND(AVERAGE(E2:E32), 0)</f>
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2575,16 +2702,16 @@
       </c>
       <c r="B37">
         <f>COUNTIF(C2:C32,"中等")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E37">
         <f>COUNTIF(D2:D32,"超时通过")</f>
-        <v>1</v>
-      </c>
-      <c r="G37" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -2595,13 +2722,13 @@
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E38">
         <f>COUNTIF(D2:D32,"提示后通过")</f>
         <v>1</v>
       </c>
-      <c r="G38" s="10"/>
+      <c r="G38" s="12"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -2612,55 +2739,55 @@
         <f>COUNTIF(D2:D32,"CV-未通过")</f>
         <v>1</v>
       </c>
-      <c r="G39" s="10"/>
+      <c r="G39" s="12"/>
     </row>
     <row r="40" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
@@ -2741,11 +2868,12 @@
       <c r="A72" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="G36:G39"/>
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="A42:G45"/>
+    <mergeCell ref="D35:E35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1 C46:C1048576 C37:C39 C6:C31">
@@ -2968,9 +3096,14 @@
     <hyperlink ref="B3" r:id="rId1" display="https://leetcode-cn.com/problems/fraction-to-recurring-decimal/" xr:uid="{8D51DA5F-1B41-41CE-B03A-EAECF1E0D932}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{0BD7FB1E-91EE-47AC-A205-64343FC13F58}"/>
     <hyperlink ref="B5" r:id="rId3" display="https://leetcode-cn.com/problems/number-of-segments-in-a-string/" xr:uid="{EA430F9D-A14D-4CDE-8359-A85C85DEB363}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://leetcode-cn.com/problems/add-two-numbers/" xr:uid="{EE888C6E-5EFF-4BBE-BC52-1C60A03B7717}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://leetcode-cn.com/problems/longest-substring-with-at-most-two-distinct-characters/" xr:uid="{3BDCA345-7E94-4E16-A0CA-C65E071326F0}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://leetcode-cn.com/problems/intersection-of-two-linked-lists/" xr:uid="{98FE7733-5C89-4AB9-8373-B2A0C1F8442E}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://leetcode-cn.com/problems/one-edit-distance/" xr:uid="{B46F5B44-2091-4837-9FAE-A908869DC99B}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://leetcode-cn.com/problems/find-peak-element/" xr:uid="{C18B2DBE-C9EE-4133-AB5F-6AB7EF5B0274}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>